<commit_message>
Cosmetic tweaks to 10y comparison
</commit_message>
<xml_diff>
--- a/data/excess_deaths_explanation/2020_vs_10y_by_date_of_occurrence.xlsx
+++ b/data/excess_deaths_explanation/2020_vs_10y_by_date_of_occurrence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\excess_deaths_explanation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4FABCA-89A8-487E-A267-581C375598FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D30206C-9441-408F-8EDC-4CA6B9660C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{99891810-AEF2-4EE9-B876-20B0CB097BF8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="raw" sheetId="1" r:id="rId1"/>
     <sheet name="screenshot" sheetId="4" r:id="rId2"/>
     <sheet name="review" sheetId="2" r:id="rId3"/>
-    <sheet name="chart" sheetId="3" r:id="rId4"/>
+    <sheet name="alt_chart" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Upper 95% confidence interval of estimate</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Check</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
   </si>
   <si>
     <t>Note</t>
@@ -96,7 +90,16 @@
     <t>Total deaths - 10 year average</t>
   </si>
   <si>
-    <t>NOT NORMAL</t>
+    <t>Above 10 year maximum</t>
+  </si>
+  <si>
+    <t>10 year min</t>
+  </si>
+  <si>
+    <t>10 year max</t>
+  </si>
+  <si>
+    <t>Total deaths - 2020 all causes</t>
   </si>
 </sst>
 </file>
@@ -263,6 +266,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8FD1F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -11445,7 +11453,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Min</c:v>
+                  <c:v>10 year min</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11811,7 +11819,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Max</c:v>
+                  <c:v>10 year max</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12412,9 +12420,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>in England + Wales 2020
-</a:t>
+              <a:t>in England + Wales 2020 compared to 2010-2019</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1200"/>
               <a:t>All figures based on date</a:t>
@@ -12480,7 +12492,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Min</c:v>
+                  <c:v>10 year min</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12827,7 +12839,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000000-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13184,27 +13196,30 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000001-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
-          <c:order val="10"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NOT NORMAL</c:v>
+                  <c:v>Above 10 year maximum</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -13378,7 +13393,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-C810-42B5-BA12-C12B56AAC589}"/>
+              <c16:uniqueId val="{00000002-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13397,8 +13412,410 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="8"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>raw!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 year min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>raw!$B$21:$BA$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>10732</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9878</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10081</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9705</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9553</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9387</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9616</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9542</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9425</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9358</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9248</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9092</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8886</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8928</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8621</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8690</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8722</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8312</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8334</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8458</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8454</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8437</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8188</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8272</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8167</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8169</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8260</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8325</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8247</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8381</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8331</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8515</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8715</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8880</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8523</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8525</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9103</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9230</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9027</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9171</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9158</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9282</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9643</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9932</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9984</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10352</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-B5F0-4126-BFE8-F7A2645621DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>raw!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 year max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>raw!$B$22:$BA$22</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>14308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13659</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12695</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12244</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12147</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12877</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12331</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11577</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11423</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11439</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10770</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10134</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10026</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9952</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10088</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9682</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9458</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9449</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9385</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9855</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9154</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9243</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9503</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9141</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9713</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8988</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9172</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9213</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9207</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9005</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9257</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9368</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9836</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9750</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9926</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10091</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10049</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10217</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10493</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10818</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10817</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11044</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11169</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>11488</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12232</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12772</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-B5F0-4126-BFE8-F7A2645621DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$18</c:f>
@@ -13759,15 +14176,23 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000003-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="6"/>
           <c:tx>
-            <c:v>Total deaths - all causes</c:v>
+            <c:strRef>
+              <c:f>raw!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total deaths - 2020 all causes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -14119,13 +14544,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000004-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="4"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$43</c:f>
@@ -14482,13 +14907,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000005-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="5"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$42</c:f>
@@ -14845,13 +15270,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000006-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="6"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$40</c:f>
@@ -15208,13 +15633,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-B83D-4EA7-B0D2-1EB53F59015E}"/>
+              <c16:uniqueId val="{00000007-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="7"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
               <c:f>raw!$A$39</c:f>
@@ -15571,381 +15996,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-B83D-4EA7-B0D2-1EB53F59015E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>raw!$B$21:$BA$21</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>10732</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10532</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10111</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9878</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9958</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10081</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9705</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9553</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9387</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9496</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9616</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9542</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9425</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9358</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9248</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9092</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9381</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8886</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8928</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8621</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8995</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>8690</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8722</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8312</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8334</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8458</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8454</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8437</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8188</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8272</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8167</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8169</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8260</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8325</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8247</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8381</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>8331</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>8515</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>8715</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>8880</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>8523</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>8525</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9103</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9230</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>9027</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>9171</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9158</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9282</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9643</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9932</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>9984</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>10352</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C810-42B5-BA12-C12B56AAC589}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>raw!$B$22:$BA$22</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="52"/>
-                <c:pt idx="0">
-                  <c:v>14308</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14653</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13640</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13659</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12695</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12221</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12244</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12256</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12147</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12877</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12331</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11577</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11423</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>11221</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10770</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10134</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10026</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9952</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10088</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9682</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9458</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9449</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9385</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9855</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9154</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9243</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9503</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9141</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9713</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8988</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9172</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9213</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9207</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9412</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9005</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9257</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9368</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>9836</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9750</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9926</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>10091</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>10049</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>10217</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>10493</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>10818</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>10817</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>11044</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>11169</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>11488</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>12232</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>12772</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C810-42B5-BA12-C12B56AAC589}"/>
+              <c16:uniqueId val="{00000008-B5F0-4126-BFE8-F7A2645621DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15962,7 +16013,7 @@
         <c:axId val="772701496"/>
         <c:axId val="772705104"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="772701496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -16009,9 +16060,10 @@
         <c:crossAx val="772705104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="772705104"/>
         <c:scaling>
@@ -16082,6 +16134,14 @@
       <c:legendPos val="t"/>
       <c:legendEntry>
         <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -20963,7 +21023,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CB0A753-FBD5-4F27-AF73-9FBA8A710D88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C37B94-EBFC-4580-93AF-47F774DC1929}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21097,7 +21157,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Created 10 Jan</a:t>
+            <a:t>Created 11 Jan</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -21284,7 +21344,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>Slightly below 5 year range, just like in Australia + NZ during Jun / Jul 2020</a:t>
+            <a:t>Slightly below 10 year range, just like in Australia + NZ during Jun / Jul 2020</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1050">
             <a:solidFill>
@@ -21774,7 +21834,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21786,7 +21846,7 @@
   <sheetData>
     <row r="1" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -23775,8 +23835,8 @@
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>2020</v>
+      <c r="A13" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13:G13" si="1">B14</f>
@@ -23988,7 +24048,7 @@
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>12431</v>
@@ -24147,7 +24207,7 @@
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -24564,7 +24624,7 @@
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18:AG18" si="4">AVERAGE(B3:B12)</f>
@@ -24777,7 +24837,7 @@
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <f>IF(B13-B22&gt;0,B13-B22,0)</f>
@@ -24990,7 +25050,7 @@
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B21" s="4">
         <f>MIN(B$3:B$12)</f>
@@ -25203,7 +25263,7 @@
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4">
         <f>MAX(B$3:B$12)</f>
@@ -25416,7 +25476,7 @@
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4">
         <f>B22-B21</f>
@@ -26055,10 +26115,10 @@
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -26114,7 +26174,7 @@
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
@@ -26275,7 +26335,7 @@
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -26436,7 +26496,7 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L33" s="10">
         <f>L32/L31</f>
@@ -26609,7 +26669,7 @@
     </row>
     <row r="35" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -26795,7 +26855,7 @@
     </row>
     <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -26981,7 +27041,7 @@
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37" s="12">
         <v>1</v>
@@ -27185,7 +27245,7 @@
     </row>
     <row r="39" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
@@ -27344,7 +27404,7 @@
     </row>
     <row r="40" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4">
         <f>B39*B37</f>
@@ -27609,7 +27669,7 @@
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B42" s="4">
         <f t="shared" ref="B42:AG42" si="57">B13-B39</f>
@@ -27819,7 +27879,7 @@
     </row>
     <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B43" s="4">
         <f t="shared" ref="B43:AG43" si="59">B13-B40</f>
@@ -28081,11 +28141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6306F4-C892-477B-B984-FAD42EE0881C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792425F7-E480-49BC-A2B2-FEBB50035096}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>